<commit_message>
aggiornamento test 450 e 451
Come da indicazioni https://github.com/ministero-salute/it-fse-support/issues/2084#issuecomment-3211129597
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ORIZZONTESPERANZAXX/FOS/23647FOS/V01/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ORIZZONTESPERANZAXX/FOS/23647FOS/V01/report-checklist.xlsx
@@ -553,13 +553,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 17" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-08-04T08:55:20+00:00 </t>
+    <t xml:space="preserve">2025-08-21T16:38:42+00:00</t>
   </si>
   <si>
     <t xml:space="preserve">719643efe906509a5debc7a9f1549b73 </t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.cfc54bb07d91645b35487178ba29443f1c88914d4dcddb75a90c6fc93e561d58.b461a849a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.cfc54bb07d91645b35487178ba29443f1c88914d4dcddb75a90c6fc93e561d58.991ad8f9d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t xml:space="preserve">OK</t>
@@ -572,13 +572,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 18" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-08-05T14:04:50+00:00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">e4f83c401bdb27333141f10e8b1f9826 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.cfc54bb07d91645b35487178ba29443f1c88914d4dcddb75a90c6fc93e561d58.70b36a74ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2025-08-21T16:44:06+00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1420f0e2ba11baa4dc54364ba7af66ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10.4.4.cfc54bb07d91645b35487178ba29443f1c88914d4dcddb75a90c6fc93e561d58.9a20d0f67e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT19_KO</t>
@@ -1254,7 +1254,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="I24 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:B996"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="I24 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2417,8 +2417,8 @@
   </sheetPr>
   <dimension ref="A1:W558"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D21" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3550,7 +3550,7 @@
         <v>123</v>
       </c>
       <c r="F23" s="32" t="n">
-        <v>45873</v>
+        <v>45890</v>
       </c>
       <c r="G23" s="32" t="s">
         <v>124</v>
@@ -3599,7 +3599,7 @@
         <v>129</v>
       </c>
       <c r="F24" s="32" t="n">
-        <v>45874</v>
+        <v>45890</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>130</v>
@@ -7518,7 +7518,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="1" sqref="I24 I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7584,7 +7584,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="1" sqref="I24 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8615,7 +8615,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I24 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>